<commit_message>
update test + eval_time BF
</commit_message>
<xml_diff>
--- a/result/eval_time.xlsx
+++ b/result/eval_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bachnt9x/Documents/GitHub/pgs/result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFEB493-24C9-2042-A291-AD84A4E5C9D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A65548-E28C-6446-8CEB-B844A19BE15C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{0A96A418-C959-8147-92A5-8E6282041EC9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="10" xr2:uid="{0A96A418-C959-8147-92A5-8E6282041EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="comp_replace" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="39">
   <si>
     <t>nComp</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>bmapreplace [s]</t>
-  </si>
-  <si>
-    <t>kpg2 + fi_cond</t>
   </si>
   <si>
     <t>lassoc_comp_breverse_nested_list [s]</t>
@@ -803,9 +800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE12618-E339-D745-ABCD-0762550117A2}">
   <dimension ref="A1:Z71"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="168" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="168" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H3" sqref="H3:H43"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,7 +885,7 @@
         <v>1.5E-5</v>
       </c>
       <c r="C3" s="41">
-        <v>2.5999999999999998E-5</v>
+        <v>4.6999999999999997E-5</v>
       </c>
       <c r="D3" s="32">
         <v>1.13E-4</v>
@@ -935,7 +932,7 @@
         <v>1.8E-5</v>
       </c>
       <c r="C4" s="41">
-        <v>2.6999999999999999E-5</v>
+        <v>4.8999999999999998E-5</v>
       </c>
       <c r="D4" s="32">
         <v>2.1900000000000001E-4</v>
@@ -982,7 +979,7 @@
         <v>1.7E-5</v>
       </c>
       <c r="C5" s="41">
-        <v>2.9E-5</v>
+        <v>5.8999999999999998E-5</v>
       </c>
       <c r="D5" s="32">
         <v>4.0499999999999998E-4</v>
@@ -1029,7 +1026,7 @@
         <v>1.8E-5</v>
       </c>
       <c r="C6" s="41">
-        <v>3.1000000000000001E-5</v>
+        <v>5.5999999999999999E-5</v>
       </c>
       <c r="D6" s="32">
         <v>7.8700000000000005E-4</v>
@@ -1076,7 +1073,7 @@
         <v>2.0999999999999999E-5</v>
       </c>
       <c r="C7" s="41">
-        <v>3.4E-5</v>
+        <v>5.7000000000000003E-5</v>
       </c>
       <c r="D7" s="32">
         <v>1.634E-3</v>
@@ -1123,7 +1120,7 @@
         <v>2.5000000000000001E-5</v>
       </c>
       <c r="C8" s="41">
-        <v>3.3000000000000003E-5</v>
+        <v>5.8999999999999998E-5</v>
       </c>
       <c r="D8" s="32">
         <v>3.238E-3</v>
@@ -1170,7 +1167,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="C9" s="41">
-        <v>3.8999999999999999E-5</v>
+        <v>5.7000000000000003E-5</v>
       </c>
       <c r="D9" s="32">
         <v>5.274E-3</v>
@@ -1217,7 +1214,7 @@
         <v>1.9000000000000001E-5</v>
       </c>
       <c r="C10" s="41">
-        <v>3.8000000000000002E-5</v>
+        <v>6.0999999999999999E-5</v>
       </c>
       <c r="D10" s="32">
         <v>9.1610000000000007E-3</v>
@@ -1264,7 +1261,7 @@
         <v>1.8E-5</v>
       </c>
       <c r="C11" s="41">
-        <v>4.0000000000000003E-5</v>
+        <v>6.6000000000000005E-5</v>
       </c>
       <c r="D11" s="32">
         <v>1.6546000000000002E-2</v>
@@ -1311,7 +1308,7 @@
         <v>1.9000000000000001E-5</v>
       </c>
       <c r="C12" s="41">
-        <v>4.5000000000000003E-5</v>
+        <v>6.8999999999999997E-5</v>
       </c>
       <c r="D12" s="32">
         <v>2.8253E-2</v>
@@ -1358,7 +1355,7 @@
         <v>1.9000000000000001E-5</v>
       </c>
       <c r="C13" s="41">
-        <v>4.8000000000000001E-5</v>
+        <v>6.9999999999999994E-5</v>
       </c>
       <c r="D13" s="32">
         <v>5.2623000000000003E-2</v>
@@ -1405,7 +1402,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="C14" s="41">
-        <v>5.0000000000000002E-5</v>
+        <v>7.2000000000000002E-5</v>
       </c>
       <c r="D14" s="32">
         <v>0.104531</v>
@@ -1452,7 +1449,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="C15" s="41">
-        <v>5.5999999999999999E-5</v>
+        <v>7.2000000000000002E-5</v>
       </c>
       <c r="D15" s="32">
         <v>0.211225</v>
@@ -1499,7 +1496,7 @@
         <v>2.0999999999999999E-5</v>
       </c>
       <c r="C16" s="41">
-        <v>6.2000000000000003E-5</v>
+        <v>7.6000000000000004E-5</v>
       </c>
       <c r="D16" s="32">
         <v>0.42589100000000002</v>
@@ -1546,7 +1543,7 @@
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="C17" s="41">
-        <v>6.7000000000000002E-5</v>
+        <v>7.8999999999999996E-5</v>
       </c>
       <c r="D17" s="32">
         <v>0.85639100000000001</v>
@@ -1593,7 +1590,7 @@
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="C18" s="41">
-        <v>7.1000000000000005E-5</v>
+        <v>8.2000000000000001E-5</v>
       </c>
       <c r="D18" s="32">
         <v>1.7145490000000001</v>
@@ -1640,7 +1637,7 @@
         <v>2.3E-5</v>
       </c>
       <c r="C19" s="41">
-        <v>7.7000000000000001E-5</v>
+        <v>8.7000000000000001E-5</v>
       </c>
       <c r="D19" s="32">
         <v>3.463889</v>
@@ -1687,7 +1684,7 @@
         <v>2.5000000000000001E-5</v>
       </c>
       <c r="C20" s="41">
-        <v>8.2999999999999998E-5</v>
+        <v>8.7000000000000001E-5</v>
       </c>
       <c r="D20" s="32">
         <v>6.8275800000000002</v>
@@ -1734,7 +1731,7 @@
         <v>2.4000000000000001E-5</v>
       </c>
       <c r="C21" s="41">
-        <v>8.0000000000000007E-5</v>
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="D21" s="32">
         <v>13.340272000000001</v>
@@ -1781,7 +1778,7 @@
         <v>2.3E-5</v>
       </c>
       <c r="C22" s="41">
-        <v>8.1000000000000004E-5</v>
+        <v>9.1000000000000003E-5</v>
       </c>
       <c r="D22" s="32">
         <v>26.941932999999999</v>
@@ -1875,7 +1872,7 @@
         <v>2.4000000000000001E-5</v>
       </c>
       <c r="C24" s="41">
-        <v>9.5000000000000005E-5</v>
+        <v>8.5000000000000006E-5</v>
       </c>
       <c r="D24" s="32">
         <v>104.913524</v>
@@ -1922,7 +1919,7 @@
         <v>2.4000000000000001E-5</v>
       </c>
       <c r="C25" s="41">
-        <v>1.02E-4</v>
+        <v>8.7000000000000001E-5</v>
       </c>
       <c r="D25" s="32">
         <v>209.92964499999999</v>
@@ -1969,7 +1966,7 @@
         <v>4.6E-5</v>
       </c>
       <c r="C26" s="41">
-        <v>3.2000000000000003E-4</v>
+        <v>1.5899999999999999E-4</v>
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="33">
@@ -2014,7 +2011,7 @@
         <v>1.4899999999999999E-4</v>
       </c>
       <c r="C27" s="41">
-        <v>2.0079999999999998E-3</v>
+        <v>4.6700000000000002E-4</v>
       </c>
       <c r="D27" s="32"/>
       <c r="E27" s="33">
@@ -2059,7 +2056,7 @@
         <v>5.3300000000000005E-4</v>
       </c>
       <c r="C28" s="41">
-        <v>1.4630000000000001E-2</v>
+        <v>1.469E-3</v>
       </c>
       <c r="D28" s="32"/>
       <c r="E28" s="33">
@@ -2104,7 +2101,7 @@
         <v>3.3409999999999998E-3</v>
       </c>
       <c r="C29" s="41">
-        <v>0.18803400000000001</v>
+        <v>7.4530000000000004E-3</v>
       </c>
       <c r="D29" s="32"/>
       <c r="E29" s="33">
@@ -2149,7 +2146,7 @@
         <v>1.3181E-2</v>
       </c>
       <c r="C30" s="41">
-        <v>1.366862</v>
+        <v>2.5572999999999999E-2</v>
       </c>
       <c r="D30" s="32"/>
       <c r="E30" s="33">
@@ -2194,7 +2191,7 @@
         <v>3.0245999999999999E-2</v>
       </c>
       <c r="C31" s="41">
-        <v>4.5900840000000001</v>
+        <v>4.9845E-2</v>
       </c>
       <c r="D31" s="32"/>
       <c r="E31" s="33">
@@ -2239,7 +2236,7 @@
         <v>5.2839999999999998E-2</v>
       </c>
       <c r="C32" s="41">
-        <v>10.637556999999999</v>
+        <v>8.6052000000000003E-2</v>
       </c>
       <c r="D32" s="32"/>
       <c r="E32" s="33">
@@ -2284,7 +2281,7 @@
         <v>8.4138000000000004E-2</v>
       </c>
       <c r="C33" s="41">
-        <v>20.978601999999999</v>
+        <v>0.13165099999999999</v>
       </c>
       <c r="D33" s="32"/>
       <c r="E33" s="33">
@@ -2329,7 +2326,7 @@
         <v>0.32829700000000001</v>
       </c>
       <c r="C34" s="41">
-        <v>172.40483399999999</v>
+        <v>0.51679799999999998</v>
       </c>
       <c r="D34" s="32"/>
       <c r="E34" s="33">
@@ -2373,7 +2370,9 @@
       <c r="B35" s="31">
         <v>1.308851</v>
       </c>
-      <c r="C35" s="41"/>
+      <c r="C35" s="41">
+        <v>2.2097479999999998</v>
+      </c>
       <c r="D35" s="32"/>
       <c r="E35" s="33">
         <v>0.45364199999999999</v>
@@ -2416,7 +2415,9 @@
       <c r="B36" s="31">
         <v>5.3511759999999997</v>
       </c>
-      <c r="C36" s="41"/>
+      <c r="C36" s="41">
+        <v>9.1069279999999999</v>
+      </c>
       <c r="D36" s="32"/>
       <c r="E36" s="33">
         <v>1.793031</v>
@@ -2459,7 +2460,9 @@
       <c r="B37" s="31">
         <v>11.777378000000001</v>
       </c>
-      <c r="C37" s="41"/>
+      <c r="C37" s="41">
+        <v>19.803684000000001</v>
+      </c>
       <c r="D37" s="32"/>
       <c r="E37" s="33">
         <v>3.8456769999999998</v>
@@ -2502,7 +2505,9 @@
       <c r="B38" s="31">
         <v>20.231997</v>
       </c>
-      <c r="C38" s="41"/>
+      <c r="C38" s="41">
+        <v>35.884129999999999</v>
+      </c>
       <c r="D38" s="32"/>
       <c r="E38" s="33">
         <v>6.8360450000000004</v>
@@ -2545,7 +2550,9 @@
       <c r="B39" s="31">
         <v>32.008606999999998</v>
       </c>
-      <c r="C39" s="41"/>
+      <c r="C39" s="41">
+        <v>57.682471</v>
+      </c>
       <c r="D39" s="32"/>
       <c r="E39" s="33">
         <v>10.543677000000001</v>
@@ -4604,7 +4611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2176A5-75DF-A044-ABD9-8458655436F1}">
   <dimension ref="A1:W73"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="168" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="168" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:H36"/>
     </sheetView>
@@ -8029,7 +8036,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
@@ -8038,7 +8045,7 @@
       <c r="G1" s="49"/>
       <c r="H1" s="50"/>
       <c r="I1" s="51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J1" s="52"/>
       <c r="K1" s="52"/>
@@ -10051,7 +10058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E16F1A3-C3C0-3C43-978B-5219F965718F}">
   <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="223" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="223" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="I22" sqref="I22"/>
     </sheetView>
@@ -13375,7 +13382,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
@@ -13384,7 +13391,7 @@
       <c r="G1" s="49"/>
       <c r="H1" s="50"/>
       <c r="I1" s="51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J1" s="52"/>
       <c r="K1" s="52"/>
@@ -17708,11 +17715,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{299A7C5B-E613-9D41-9E92-86EAED0A2A4D}">
-  <dimension ref="A1:W73"/>
+  <dimension ref="A1:V73"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="168" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="150" zoomScaleNormal="168" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H36" sqref="H36"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17720,7 +17727,7 @@
     <col min="1" max="16384" width="15.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="54" t="s">
         <v>32</v>
       </c>
@@ -17735,9 +17742,8 @@
       <c r="K1" s="21"/>
       <c r="L1" s="21"/>
       <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-    </row>
-    <row r="2" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -17762,16 +17768,13 @@
       <c r="H2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="47" t="s">
-        <v>33</v>
-      </c>
+      <c r="I2" s="20"/>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
       <c r="L2" s="20"/>
       <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>10</v>
       </c>
@@ -17779,7 +17782,7 @@
         <v>5.3000000000000001E-5</v>
       </c>
       <c r="C3" s="41">
-        <v>5.8E-5</v>
+        <v>6.3999999999999997E-5</v>
       </c>
       <c r="D3" s="32">
         <v>1.536E-3</v>
@@ -17794,18 +17797,15 @@
         <v>5.7000000000000003E-5</v>
       </c>
       <c r="H3" s="35">
-        <v>3.8000000000000002E-5</v>
-      </c>
-      <c r="I3" s="44">
-        <v>6.7000000000000002E-5</v>
-      </c>
+        <v>5.3999999999999998E-5</v>
+      </c>
+      <c r="I3" s="44"/>
       <c r="J3" s="44"/>
       <c r="K3" s="44"/>
       <c r="L3" s="44"/>
       <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>11</v>
       </c>
@@ -17813,7 +17813,7 @@
         <v>5.8E-5</v>
       </c>
       <c r="C4" s="41">
-        <v>6.2000000000000003E-5</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="D4" s="32">
         <v>3.3270000000000001E-3</v>
@@ -17828,18 +17828,15 @@
         <v>6.0999999999999999E-5</v>
       </c>
       <c r="H4" s="35">
-        <v>4.3000000000000002E-5</v>
-      </c>
-      <c r="I4" s="44">
-        <v>7.7000000000000001E-5</v>
-      </c>
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="I4" s="44"/>
       <c r="J4" s="44"/>
       <c r="K4" s="44"/>
       <c r="L4" s="44"/>
       <c r="M4" s="44"/>
-      <c r="N4" s="44"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>12</v>
       </c>
@@ -17847,7 +17844,7 @@
         <v>6.6000000000000005E-5</v>
       </c>
       <c r="C5" s="41">
-        <v>7.6000000000000004E-5</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="D5" s="32">
         <v>5.7730000000000004E-3</v>
@@ -17862,18 +17859,15 @@
         <v>6.9999999999999994E-5</v>
       </c>
       <c r="H5" s="35">
-        <v>4.3999999999999999E-5</v>
-      </c>
-      <c r="I5" s="44">
-        <v>7.7999999999999999E-5</v>
-      </c>
+        <v>4.6999999999999997E-5</v>
+      </c>
+      <c r="I5" s="44"/>
       <c r="J5" s="44"/>
       <c r="K5" s="44"/>
       <c r="L5" s="44"/>
       <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>13</v>
       </c>
@@ -17881,7 +17875,7 @@
         <v>7.4999999999999993E-5</v>
       </c>
       <c r="C6" s="41">
-        <v>7.7999999999999999E-5</v>
+        <v>8.5000000000000006E-5</v>
       </c>
       <c r="D6" s="32">
         <v>1.0748000000000001E-2</v>
@@ -17896,18 +17890,15 @@
         <v>7.4999999999999993E-5</v>
       </c>
       <c r="H6" s="35">
-        <v>4.6E-5</v>
-      </c>
-      <c r="I6" s="44">
-        <v>9.2E-5</v>
-      </c>
+        <v>5.3999999999999998E-5</v>
+      </c>
+      <c r="I6" s="44"/>
       <c r="J6" s="44"/>
       <c r="K6" s="44"/>
       <c r="L6" s="44"/>
       <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>14</v>
       </c>
@@ -17915,7 +17906,7 @@
         <v>8.2000000000000001E-5</v>
       </c>
       <c r="C7" s="41">
-        <v>8.2000000000000001E-5</v>
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="D7" s="32">
         <v>1.8270999999999999E-2</v>
@@ -17930,18 +17921,15 @@
         <v>8.2000000000000001E-5</v>
       </c>
       <c r="H7" s="35">
-        <v>4.8999999999999998E-5</v>
-      </c>
-      <c r="I7" s="44">
-        <v>9.5000000000000005E-5</v>
-      </c>
+        <v>6.3E-5</v>
+      </c>
+      <c r="I7" s="44"/>
       <c r="J7" s="44"/>
       <c r="K7" s="44"/>
       <c r="L7" s="44"/>
       <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>15</v>
       </c>
@@ -17949,7 +17937,7 @@
         <v>9.0000000000000006E-5</v>
       </c>
       <c r="C8" s="41">
-        <v>8.7999999999999998E-5</v>
+        <v>9.6000000000000002E-5</v>
       </c>
       <c r="D8" s="32">
         <v>3.1149E-2</v>
@@ -17964,18 +17952,15 @@
         <v>9.1000000000000003E-5</v>
       </c>
       <c r="H8" s="35">
-        <v>4.8000000000000001E-5</v>
-      </c>
-      <c r="I8" s="44">
-        <v>1.08E-4</v>
-      </c>
+        <v>6.0999999999999999E-5</v>
+      </c>
+      <c r="I8" s="44"/>
       <c r="J8" s="44"/>
       <c r="K8" s="44"/>
       <c r="L8" s="44"/>
       <c r="M8" s="44"/>
-      <c r="N8" s="44"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>16</v>
       </c>
@@ -17983,7 +17968,7 @@
         <v>1E-4</v>
       </c>
       <c r="C9" s="41">
-        <v>1.01E-4</v>
+        <v>1.05E-4</v>
       </c>
       <c r="D9" s="32">
         <v>5.7062000000000002E-2</v>
@@ -17998,18 +17983,15 @@
         <v>1.02E-4</v>
       </c>
       <c r="H9" s="35">
-        <v>5.3000000000000001E-5</v>
-      </c>
-      <c r="I9" s="44">
-        <v>1.08E-4</v>
-      </c>
+        <v>6.0999999999999999E-5</v>
+      </c>
+      <c r="I9" s="44"/>
       <c r="J9" s="44"/>
       <c r="K9" s="44"/>
       <c r="L9" s="44"/>
       <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>17</v>
       </c>
@@ -18017,7 +17999,7 @@
         <v>1.05E-4</v>
       </c>
       <c r="C10" s="41">
-        <v>9.7E-5</v>
+        <v>1.0399999999999999E-4</v>
       </c>
       <c r="D10" s="32">
         <v>0.11377900000000001</v>
@@ -18032,18 +18014,15 @@
         <v>1.08E-4</v>
       </c>
       <c r="H10" s="35">
-        <v>5.7000000000000003E-5</v>
-      </c>
-      <c r="I10" s="44">
-        <v>1.21E-4</v>
-      </c>
+        <v>6.0999999999999999E-5</v>
+      </c>
+      <c r="I10" s="44"/>
       <c r="J10" s="44"/>
       <c r="K10" s="44"/>
       <c r="L10" s="44"/>
       <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>18</v>
       </c>
@@ -18051,7 +18030,7 @@
         <v>1.11E-4</v>
       </c>
       <c r="C11" s="41">
-        <v>1.06E-4</v>
+        <v>1.0900000000000001E-4</v>
       </c>
       <c r="D11" s="32">
         <v>0.22658800000000001</v>
@@ -18066,18 +18045,15 @@
         <v>1.22E-4</v>
       </c>
       <c r="H11" s="35">
-        <v>5.3999999999999998E-5</v>
-      </c>
-      <c r="I11" s="44">
-        <v>1.2400000000000001E-4</v>
-      </c>
+        <v>6.3999999999999997E-5</v>
+      </c>
+      <c r="I11" s="44"/>
       <c r="J11" s="44"/>
       <c r="K11" s="44"/>
       <c r="L11" s="44"/>
       <c r="M11" s="44"/>
-      <c r="N11" s="44"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>19</v>
       </c>
@@ -18085,7 +18061,7 @@
         <v>1.18E-4</v>
       </c>
       <c r="C12" s="41">
-        <v>1.02E-4</v>
+        <v>1.05E-4</v>
       </c>
       <c r="D12" s="32">
         <v>0.45527800000000002</v>
@@ -18100,18 +18076,15 @@
         <v>1.26E-4</v>
       </c>
       <c r="H12" s="35">
-        <v>5.3000000000000001E-5</v>
-      </c>
-      <c r="I12" s="44">
-        <v>1.3100000000000001E-4</v>
-      </c>
+        <v>6.6000000000000005E-5</v>
+      </c>
+      <c r="I12" s="44"/>
       <c r="J12" s="44"/>
       <c r="K12" s="44"/>
       <c r="L12" s="44"/>
       <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>20</v>
       </c>
@@ -18134,18 +18107,15 @@
         <v>1.34E-4</v>
       </c>
       <c r="H13" s="35">
-        <v>5.5999999999999999E-5</v>
-      </c>
-      <c r="I13" s="44">
-        <v>1.37E-4</v>
-      </c>
+        <v>6.4999999999999994E-5</v>
+      </c>
+      <c r="I13" s="44"/>
       <c r="J13" s="44"/>
       <c r="K13" s="44"/>
       <c r="L13" s="44"/>
       <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>21</v>
       </c>
@@ -18168,18 +18138,15 @@
         <v>1.3200000000000001E-4</v>
       </c>
       <c r="H14" s="35">
-        <v>6.0000000000000002E-5</v>
-      </c>
-      <c r="I14" s="44">
-        <v>1.4999999999999999E-4</v>
-      </c>
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="I14" s="44"/>
       <c r="J14" s="44"/>
       <c r="K14" s="44"/>
       <c r="L14" s="44"/>
       <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>22</v>
       </c>
@@ -18187,7 +18154,7 @@
         <v>1.46E-4</v>
       </c>
       <c r="C15" s="41">
-        <v>1.12E-4</v>
+        <v>1.16E-4</v>
       </c>
       <c r="D15" s="32">
         <v>3.7175799999999999</v>
@@ -18202,18 +18169,15 @@
         <v>1.47E-4</v>
       </c>
       <c r="H15" s="35">
-        <v>5.7000000000000003E-5</v>
-      </c>
-      <c r="I15" s="44">
-        <v>1.6100000000000001E-4</v>
-      </c>
+        <v>6.6000000000000005E-5</v>
+      </c>
+      <c r="I15" s="44"/>
       <c r="J15" s="44"/>
       <c r="K15" s="44"/>
       <c r="L15" s="44"/>
       <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>23</v>
       </c>
@@ -18221,7 +18185,7 @@
         <v>1.5899999999999999E-4</v>
       </c>
       <c r="C16" s="41">
-        <v>1.2799999999999999E-4</v>
+        <v>1.3200000000000001E-4</v>
       </c>
       <c r="D16" s="32">
         <v>7.2312909999999997</v>
@@ -18236,18 +18200,15 @@
         <v>1.55E-4</v>
       </c>
       <c r="H16" s="35">
-        <v>6.2000000000000003E-5</v>
-      </c>
-      <c r="I16" s="44">
-        <v>1.7799999999999999E-4</v>
-      </c>
+        <v>6.6000000000000005E-5</v>
+      </c>
+      <c r="I16" s="44"/>
       <c r="J16" s="44"/>
       <c r="K16" s="44"/>
       <c r="L16" s="44"/>
       <c r="M16" s="44"/>
-      <c r="N16" s="44"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>24</v>
       </c>
@@ -18255,7 +18216,7 @@
         <v>1.6899999999999999E-4</v>
       </c>
       <c r="C17" s="41">
-        <v>1.2899999999999999E-4</v>
+        <v>1.36E-4</v>
       </c>
       <c r="D17" s="32">
         <v>14.31325</v>
@@ -18270,18 +18231,15 @@
         <v>1.8000000000000001E-4</v>
       </c>
       <c r="H17" s="35">
-        <v>6.6000000000000005E-5</v>
-      </c>
-      <c r="I17" s="44">
-        <v>1.8699999999999999E-4</v>
-      </c>
+        <v>7.1000000000000005E-5</v>
+      </c>
+      <c r="I17" s="44"/>
       <c r="J17" s="44"/>
       <c r="K17" s="44"/>
       <c r="L17" s="44"/>
       <c r="M17" s="44"/>
-      <c r="N17" s="44"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>25</v>
       </c>
@@ -18289,7 +18247,7 @@
         <v>1.7200000000000001E-4</v>
       </c>
       <c r="C18" s="41">
-        <v>1.37E-4</v>
+        <v>1.4100000000000001E-4</v>
       </c>
       <c r="D18" s="32">
         <v>28.965609000000001</v>
@@ -18304,18 +18262,15 @@
         <v>1.7200000000000001E-4</v>
       </c>
       <c r="H18" s="35">
-        <v>6.3999999999999997E-5</v>
-      </c>
-      <c r="I18" s="44">
-        <v>1.9599999999999999E-4</v>
-      </c>
+        <v>8.1000000000000004E-5</v>
+      </c>
+      <c r="I18" s="44"/>
       <c r="J18" s="44"/>
       <c r="K18" s="44"/>
       <c r="L18" s="44"/>
       <c r="M18" s="44"/>
-      <c r="N18" s="44"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>26</v>
       </c>
@@ -18323,7 +18278,7 @@
         <v>1.65E-4</v>
       </c>
       <c r="C19" s="41">
-        <v>1.36E-4</v>
+        <v>1.47E-4</v>
       </c>
       <c r="D19" s="32">
         <v>57.661036000000003</v>
@@ -18338,18 +18293,15 @@
         <v>1.83E-4</v>
       </c>
       <c r="H19" s="35">
-        <v>6.0999999999999999E-5</v>
-      </c>
-      <c r="I19" s="44">
-        <v>2.3800000000000001E-4</v>
-      </c>
+        <v>7.2000000000000002E-5</v>
+      </c>
+      <c r="I19" s="44"/>
       <c r="J19" s="44"/>
       <c r="K19" s="44"/>
       <c r="L19" s="44"/>
       <c r="M19" s="44"/>
-      <c r="N19" s="44"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>27</v>
       </c>
@@ -18357,7 +18309,7 @@
         <v>1.6899999999999999E-4</v>
       </c>
       <c r="C20" s="41">
-        <v>1.3899999999999999E-4</v>
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="33">
@@ -18370,18 +18322,15 @@
         <v>1.9599999999999999E-4</v>
       </c>
       <c r="H20" s="35">
-        <v>5.8999999999999998E-5</v>
-      </c>
-      <c r="I20" s="44">
-        <v>2.23E-4</v>
-      </c>
+        <v>7.3999999999999996E-5</v>
+      </c>
+      <c r="I20" s="44"/>
       <c r="J20" s="44"/>
       <c r="K20" s="44"/>
       <c r="L20" s="44"/>
       <c r="M20" s="44"/>
-      <c r="N20" s="44"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>28</v>
       </c>
@@ -18389,7 +18338,7 @@
         <v>1.8200000000000001E-4</v>
       </c>
       <c r="C21" s="41">
-        <v>1.4300000000000001E-4</v>
+        <v>1.5200000000000001E-4</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="33">
@@ -18402,18 +18351,15 @@
         <v>1.8599999999999999E-4</v>
       </c>
       <c r="H21" s="35">
-        <v>6.0000000000000002E-5</v>
-      </c>
-      <c r="I21" s="44">
-        <v>2.1000000000000001E-4</v>
-      </c>
+        <v>7.6000000000000004E-5</v>
+      </c>
+      <c r="I21" s="44"/>
       <c r="J21" s="44"/>
       <c r="K21" s="44"/>
       <c r="L21" s="44"/>
       <c r="M21" s="44"/>
-      <c r="N21" s="44"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>29</v>
       </c>
@@ -18421,7 +18367,7 @@
         <v>1.93E-4</v>
       </c>
       <c r="C22" s="41">
-        <v>1.4799999999999999E-4</v>
+        <v>1.54E-4</v>
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="33">
@@ -18434,18 +18380,15 @@
         <v>1.8200000000000001E-4</v>
       </c>
       <c r="H22" s="35">
-        <v>6.0999999999999999E-5</v>
-      </c>
-      <c r="I22" s="44">
-        <v>2.0799999999999999E-4</v>
-      </c>
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="I22" s="44"/>
       <c r="J22" s="44"/>
       <c r="K22" s="44"/>
       <c r="L22" s="44"/>
       <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>30</v>
       </c>
@@ -18453,7 +18396,7 @@
         <v>2.0699999999999999E-4</v>
       </c>
       <c r="C23" s="41">
-        <v>1.4300000000000001E-4</v>
+        <v>1.4100000000000001E-4</v>
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="33">
@@ -18466,18 +18409,15 @@
         <v>1.94E-4</v>
       </c>
       <c r="H23" s="35">
-        <v>6.2000000000000003E-5</v>
-      </c>
-      <c r="I23" s="44">
-        <v>2.1900000000000001E-4</v>
-      </c>
+        <v>8.6000000000000003E-5</v>
+      </c>
+      <c r="I23" s="44"/>
       <c r="J23" s="44"/>
       <c r="K23" s="44"/>
       <c r="L23" s="44"/>
       <c r="M23" s="44"/>
-      <c r="N23" s="44"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>31</v>
       </c>
@@ -18485,7 +18425,7 @@
         <v>2.1599999999999999E-4</v>
       </c>
       <c r="C24" s="41">
-        <v>1.2899999999999999E-4</v>
+        <v>1.36E-4</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="33">
@@ -18498,18 +18438,15 @@
         <v>2.02E-4</v>
       </c>
       <c r="H24" s="35">
-        <v>6.6000000000000005E-5</v>
-      </c>
-      <c r="I24" s="44">
-        <v>2.4699999999999999E-4</v>
-      </c>
+        <v>8.6000000000000003E-5</v>
+      </c>
+      <c r="I24" s="44"/>
       <c r="J24" s="44"/>
       <c r="K24" s="44"/>
       <c r="L24" s="44"/>
       <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>32</v>
       </c>
@@ -18517,7 +18454,7 @@
         <v>2.3000000000000001E-4</v>
       </c>
       <c r="C25" s="41">
-        <v>1.3300000000000001E-4</v>
+        <v>1.4100000000000001E-4</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="33">
@@ -18530,18 +18467,15 @@
         <v>2.23E-4</v>
       </c>
       <c r="H25" s="35">
-        <v>6.3999999999999997E-5</v>
-      </c>
-      <c r="I25" s="44">
-        <v>2.5099999999999998E-4</v>
-      </c>
+        <v>8.5000000000000006E-5</v>
+      </c>
+      <c r="I25" s="44"/>
       <c r="J25" s="44"/>
       <c r="K25" s="44"/>
       <c r="L25" s="44"/>
       <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>50</v>
       </c>
@@ -18549,7 +18483,7 @@
         <v>5.3799999999999996E-4</v>
       </c>
       <c r="C26" s="41">
-        <v>2.2000000000000001E-4</v>
+        <v>2.2800000000000001E-4</v>
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="33">
@@ -18562,18 +18496,15 @@
         <v>4.9700000000000005E-4</v>
       </c>
       <c r="H26" s="35">
-        <v>1E-4</v>
-      </c>
-      <c r="I26" s="44">
-        <v>5.5900000000000004E-4</v>
-      </c>
+        <v>1.4899999999999999E-4</v>
+      </c>
+      <c r="I26" s="44"/>
       <c r="J26" s="44"/>
       <c r="K26" s="44"/>
       <c r="L26" s="44"/>
       <c r="M26" s="44"/>
-      <c r="N26" s="44"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>100</v>
       </c>
@@ -18581,7 +18512,7 @@
         <v>2.1180000000000001E-3</v>
       </c>
       <c r="C27" s="41">
-        <v>4.84E-4</v>
+        <v>4.6299999999999998E-4</v>
       </c>
       <c r="D27" s="32"/>
       <c r="E27" s="33">
@@ -18594,18 +18525,15 @@
         <v>1.8469999999999999E-3</v>
       </c>
       <c r="H27" s="35">
-        <v>2.13E-4</v>
-      </c>
-      <c r="I27" s="44">
-        <v>2.1210000000000001E-3</v>
-      </c>
+        <v>3.0200000000000002E-4</v>
+      </c>
+      <c r="I27" s="44"/>
       <c r="J27" s="44"/>
       <c r="K27" s="44"/>
       <c r="L27" s="44"/>
       <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>200</v>
       </c>
@@ -18613,7 +18541,7 @@
         <v>7.8860000000000006E-3</v>
       </c>
       <c r="C28" s="41">
-        <v>9.0600000000000001E-4</v>
+        <v>9.2299999999999999E-4</v>
       </c>
       <c r="D28" s="32"/>
       <c r="E28" s="33">
@@ -18626,18 +18554,15 @@
         <v>6.6150000000000002E-3</v>
       </c>
       <c r="H28" s="35">
-        <v>4.0299999999999998E-4</v>
-      </c>
-      <c r="I28" s="44">
-        <v>6.9769999999999997E-3</v>
-      </c>
+        <v>5.31E-4</v>
+      </c>
+      <c r="I28" s="44"/>
       <c r="J28" s="44"/>
       <c r="K28" s="44"/>
       <c r="L28" s="44"/>
       <c r="M28" s="44"/>
-      <c r="N28" s="44"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>500</v>
       </c>
@@ -18645,7 +18570,7 @@
         <v>4.5746000000000002E-2</v>
       </c>
       <c r="C29" s="41">
-        <v>2.1069999999999999E-3</v>
+        <v>2.2139999999999998E-3</v>
       </c>
       <c r="D29" s="32"/>
       <c r="E29" s="33">
@@ -18658,18 +18583,15 @@
         <v>3.9286000000000001E-2</v>
       </c>
       <c r="H29" s="35">
-        <v>9.9400000000000009E-4</v>
-      </c>
-      <c r="I29" s="44">
-        <v>4.0605000000000002E-2</v>
-      </c>
+        <v>1.426E-3</v>
+      </c>
+      <c r="I29" s="44"/>
       <c r="J29" s="44"/>
       <c r="K29" s="44"/>
       <c r="L29" s="44"/>
       <c r="M29" s="44"/>
-      <c r="N29" s="44"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>1000</v>
       </c>
@@ -18677,7 +18599,7 @@
         <v>0.179225</v>
       </c>
       <c r="C30" s="41">
-        <v>4.2079999999999999E-3</v>
+        <v>4.4289999999999998E-3</v>
       </c>
       <c r="D30" s="32"/>
       <c r="E30" s="33">
@@ -18690,18 +18612,15 @@
         <v>0.15382799999999999</v>
       </c>
       <c r="H30" s="35">
-        <v>2.1380000000000001E-3</v>
-      </c>
-      <c r="I30" s="44">
-        <v>0.156278</v>
-      </c>
+        <v>3.637E-3</v>
+      </c>
+      <c r="I30" s="44"/>
       <c r="J30" s="44"/>
       <c r="K30" s="44"/>
       <c r="L30" s="44"/>
       <c r="M30" s="44"/>
-      <c r="N30" s="44"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>1500</v>
       </c>
@@ -18709,7 +18628,7 @@
         <v>0.40684999999999999</v>
       </c>
       <c r="C31" s="41">
-        <v>6.8240000000000002E-3</v>
+        <v>7.0889999999999998E-3</v>
       </c>
       <c r="D31" s="32"/>
       <c r="E31" s="33">
@@ -18722,18 +18641,15 @@
         <v>0.33998800000000001</v>
       </c>
       <c r="H31" s="35">
-        <v>3.8739999999999998E-3</v>
-      </c>
-      <c r="I31" s="44">
-        <v>0.34078399999999998</v>
-      </c>
+        <v>4.9459999999999999E-3</v>
+      </c>
+      <c r="I31" s="44"/>
       <c r="J31" s="44"/>
       <c r="K31" s="44"/>
       <c r="L31" s="44"/>
       <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>2000</v>
       </c>
@@ -18741,7 +18657,7 @@
         <v>0.72748400000000002</v>
       </c>
       <c r="C32" s="41">
-        <v>8.5000000000000006E-3</v>
+        <v>9.103E-3</v>
       </c>
       <c r="D32" s="32"/>
       <c r="E32" s="33">
@@ -18754,18 +18670,15 @@
         <v>0.62682599999999999</v>
       </c>
       <c r="H32" s="35">
-        <v>5.6049999999999997E-3</v>
-      </c>
-      <c r="I32" s="44">
-        <v>0.70856699999999995</v>
-      </c>
+        <v>7.4180000000000001E-3</v>
+      </c>
+      <c r="I32" s="44"/>
       <c r="J32" s="44"/>
       <c r="K32" s="44"/>
       <c r="L32" s="44"/>
       <c r="M32" s="44"/>
-      <c r="N32" s="44"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>2500</v>
       </c>
@@ -18773,7 +18686,7 @@
         <v>1.159286</v>
       </c>
       <c r="C33" s="41">
-        <v>1.0194999999999999E-2</v>
+        <v>1.2545000000000001E-2</v>
       </c>
       <c r="D33" s="32"/>
       <c r="E33" s="33">
@@ -18786,18 +18699,15 @@
         <v>1.0069250000000001</v>
       </c>
       <c r="H33" s="35">
-        <v>8.8579999999999996E-3</v>
-      </c>
-      <c r="I33" s="44">
-        <v>1.06609</v>
-      </c>
+        <v>9.5119999999999996E-3</v>
+      </c>
+      <c r="I33" s="44"/>
       <c r="J33" s="44"/>
       <c r="K33" s="44"/>
       <c r="L33" s="44"/>
       <c r="M33" s="44"/>
-      <c r="N33" s="44"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>3000</v>
       </c>
@@ -18805,7 +18715,7 @@
         <v>1.7674129999999999</v>
       </c>
       <c r="C34" s="41">
-        <v>1.575E-2</v>
+        <v>1.9049E-2</v>
       </c>
       <c r="D34" s="32"/>
       <c r="E34" s="33">
@@ -18818,18 +18728,15 @@
         <v>1.5081850000000001</v>
       </c>
       <c r="H34" s="35">
-        <v>9.1900000000000003E-3</v>
-      </c>
-      <c r="I34" s="44">
-        <v>1.765385</v>
-      </c>
+        <v>9.8189999999999996E-3</v>
+      </c>
+      <c r="I34" s="44"/>
       <c r="J34" s="44"/>
       <c r="K34" s="44"/>
       <c r="L34" s="44"/>
       <c r="M34" s="44"/>
-      <c r="N34" s="44"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>5000</v>
       </c>
@@ -18837,7 +18744,7 @@
         <v>5.1500269999999997</v>
       </c>
       <c r="C35" s="41">
-        <v>2.3605999999999999E-2</v>
+        <v>3.1428999999999999E-2</v>
       </c>
       <c r="D35" s="32"/>
       <c r="E35" s="33">
@@ -18850,18 +18757,15 @@
         <v>4.3984449999999997</v>
       </c>
       <c r="H35" s="35">
-        <v>1.8296E-2</v>
-      </c>
-      <c r="I35" s="44">
-        <v>5.317329</v>
-      </c>
+        <v>1.9251999999999998E-2</v>
+      </c>
+      <c r="I35" s="44"/>
       <c r="J35" s="44"/>
       <c r="K35" s="44"/>
       <c r="L35" s="44"/>
       <c r="M35" s="44"/>
-      <c r="N35" s="44"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>10000</v>
       </c>
@@ -18869,7 +18773,7 @@
         <v>23.346927000000001</v>
       </c>
       <c r="C36" s="41">
-        <v>4.7646000000000001E-2</v>
+        <v>5.3596999999999999E-2</v>
       </c>
       <c r="D36" s="32"/>
       <c r="E36" s="33">
@@ -18882,18 +18786,15 @@
         <v>31.583176999999999</v>
       </c>
       <c r="H36" s="35">
-        <v>4.5405000000000001E-2</v>
-      </c>
-      <c r="I36" s="44">
-        <v>34.186042999999998</v>
-      </c>
+        <v>4.4274000000000001E-2</v>
+      </c>
+      <c r="I36" s="44"/>
       <c r="J36" s="44"/>
       <c r="K36" s="44"/>
       <c r="L36" s="44"/>
       <c r="M36" s="44"/>
-      <c r="N36" s="44"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>20000</v>
       </c>
@@ -18901,7 +18802,7 @@
         <v>111.146433</v>
       </c>
       <c r="C37" s="41">
-        <v>0.10918</v>
+        <v>0.121602</v>
       </c>
       <c r="D37" s="32"/>
       <c r="E37" s="33" t="s">
@@ -18913,24 +18814,19 @@
       <c r="G37" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="35" t="s">
-        <v>4</v>
-      </c>
+      <c r="H37" s="35"/>
       <c r="I37" s="44"/>
       <c r="J37" s="44"/>
       <c r="K37" s="44"/>
       <c r="L37" s="44"/>
       <c r="M37" s="44"/>
-      <c r="N37" s="44"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>30000</v>
       </c>
       <c r="B38" s="31"/>
-      <c r="C38" s="41" t="s">
-        <v>4</v>
-      </c>
+      <c r="C38" s="41"/>
       <c r="D38" s="32"/>
       <c r="E38" s="33"/>
       <c r="F38" s="34"/>
@@ -18941,9 +18837,8 @@
       <c r="K38" s="44"/>
       <c r="L38" s="44"/>
       <c r="M38" s="44"/>
-      <c r="N38" s="44"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>40000</v>
       </c>
@@ -18959,9 +18854,8 @@
       <c r="K39" s="44"/>
       <c r="L39" s="44"/>
       <c r="M39" s="44"/>
-      <c r="N39" s="44"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>50000</v>
       </c>
@@ -18977,9 +18871,8 @@
       <c r="K40" s="44"/>
       <c r="L40" s="44"/>
       <c r="M40" s="44"/>
-      <c r="N40" s="44"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>60000</v>
       </c>
@@ -18995,9 +18888,8 @@
       <c r="K41" s="44"/>
       <c r="L41" s="44"/>
       <c r="M41" s="44"/>
-      <c r="N41" s="44"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>70000</v>
       </c>
@@ -19013,9 +18905,8 @@
       <c r="K42" s="44"/>
       <c r="L42" s="44"/>
       <c r="M42" s="44"/>
-      <c r="N42" s="44"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>80000</v>
       </c>
@@ -19031,9 +18922,8 @@
       <c r="K43" s="44"/>
       <c r="L43" s="44"/>
       <c r="M43" s="44"/>
-      <c r="N43" s="44"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>90000</v>
       </c>
@@ -19049,9 +18939,8 @@
       <c r="K44" s="44"/>
       <c r="L44" s="44"/>
       <c r="M44" s="44"/>
-      <c r="N44" s="44"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>100000</v>
       </c>
@@ -19067,9 +18956,8 @@
       <c r="K45" s="44"/>
       <c r="L45" s="44"/>
       <c r="M45" s="44"/>
-      <c r="N45" s="44"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="25" t="s">
         <v>4</v>
       </c>
@@ -19085,12 +18973,12 @@
       <c r="K46" s="23"/>
       <c r="L46" s="23"/>
       <c r="M46" s="23"/>
-      <c r="N46" s="23"/>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="M50" s="21"/>
       <c r="N50" s="21"/>
       <c r="O50" s="21"/>
       <c r="P50" s="21"/>
@@ -19100,12 +18988,12 @@
       <c r="T50" s="21"/>
       <c r="U50" s="21"/>
       <c r="V50" s="21"/>
-      <c r="W50" s="21"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="M51" s="20"/>
       <c r="N51" s="20"/>
       <c r="O51" s="20"/>
       <c r="P51" s="20"/>
@@ -19115,289 +19003,288 @@
       <c r="T51" s="20"/>
       <c r="U51" s="20"/>
       <c r="V51" s="20"/>
-      <c r="W51" s="20"/>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="M52" s="23"/>
       <c r="N52" s="23"/>
-      <c r="O52" s="23"/>
-      <c r="P52" s="22"/>
-      <c r="Q52" s="23"/>
-      <c r="R52" s="22"/>
+      <c r="O52" s="22"/>
+      <c r="P52" s="23"/>
+      <c r="Q52" s="22"/>
+      <c r="R52" s="23"/>
       <c r="S52" s="23"/>
-      <c r="T52" s="23"/>
-      <c r="U52" s="22"/>
-      <c r="V52" s="23"/>
-      <c r="W52" s="22"/>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T52" s="22"/>
+      <c r="U52" s="23"/>
+      <c r="V52" s="22"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="M53" s="23"/>
       <c r="N53" s="23"/>
-      <c r="O53" s="23"/>
-      <c r="P53" s="22"/>
-      <c r="Q53" s="23"/>
-      <c r="R53" s="22"/>
+      <c r="O53" s="22"/>
+      <c r="P53" s="23"/>
+      <c r="Q53" s="22"/>
+      <c r="R53" s="23"/>
       <c r="S53" s="23"/>
-      <c r="T53" s="23"/>
-      <c r="U53" s="22"/>
-      <c r="V53" s="23"/>
-      <c r="W53" s="22"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T53" s="22"/>
+      <c r="U53" s="23"/>
+      <c r="V53" s="22"/>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="18" t="s">
         <v>8</v>
       </c>
+      <c r="M54" s="23"/>
       <c r="N54" s="23"/>
-      <c r="O54" s="23"/>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="23"/>
-      <c r="R54" s="22"/>
+      <c r="O54" s="22"/>
+      <c r="P54" s="23"/>
+      <c r="Q54" s="22"/>
+      <c r="R54" s="23"/>
       <c r="S54" s="23"/>
-      <c r="T54" s="23"/>
-      <c r="U54" s="22"/>
-      <c r="V54" s="23"/>
-      <c r="W54" s="22"/>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T54" s="22"/>
+      <c r="U54" s="23"/>
+      <c r="V54" s="22"/>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="M55" s="23"/>
       <c r="N55" s="23"/>
-      <c r="O55" s="23"/>
-      <c r="P55" s="22"/>
-      <c r="Q55" s="23"/>
-      <c r="R55" s="22"/>
+      <c r="O55" s="22"/>
+      <c r="P55" s="23"/>
+      <c r="Q55" s="22"/>
+      <c r="R55" s="23"/>
       <c r="S55" s="23"/>
-      <c r="T55" s="23"/>
-      <c r="U55" s="22"/>
-      <c r="V55" s="23"/>
-      <c r="W55" s="22"/>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T55" s="22"/>
+      <c r="U55" s="23"/>
+      <c r="V55" s="22"/>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M56" s="23"/>
       <c r="N56" s="23"/>
-      <c r="O56" s="23"/>
-      <c r="P56" s="22"/>
-      <c r="Q56" s="23"/>
-      <c r="R56" s="22"/>
+      <c r="O56" s="22"/>
+      <c r="P56" s="23"/>
+      <c r="Q56" s="22"/>
+      <c r="R56" s="23"/>
       <c r="S56" s="23"/>
-      <c r="T56" s="23"/>
-      <c r="U56" s="22"/>
-      <c r="V56" s="23"/>
-      <c r="W56" s="22"/>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T56" s="22"/>
+      <c r="U56" s="23"/>
+      <c r="V56" s="22"/>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
         <v>22</v>
       </c>
+      <c r="M57" s="23"/>
       <c r="N57" s="23"/>
-      <c r="O57" s="23"/>
-      <c r="P57" s="22"/>
-      <c r="Q57" s="23"/>
-      <c r="R57" s="22"/>
+      <c r="O57" s="22"/>
+      <c r="P57" s="23"/>
+      <c r="Q57" s="22"/>
+      <c r="R57" s="23"/>
       <c r="S57" s="23"/>
-      <c r="T57" s="23"/>
-      <c r="U57" s="22"/>
-      <c r="V57" s="23"/>
-      <c r="W57" s="22"/>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T57" s="22"/>
+      <c r="U57" s="23"/>
+      <c r="V57" s="22"/>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M58" s="23"/>
       <c r="N58" s="23"/>
-      <c r="O58" s="23"/>
-      <c r="P58" s="22"/>
-      <c r="Q58" s="23"/>
-      <c r="R58" s="22"/>
+      <c r="O58" s="22"/>
+      <c r="P58" s="23"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="23"/>
       <c r="S58" s="23"/>
-      <c r="T58" s="23"/>
-      <c r="U58" s="22"/>
-      <c r="V58" s="23"/>
-      <c r="W58" s="22"/>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T58" s="22"/>
+      <c r="U58" s="23"/>
+      <c r="V58" s="22"/>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M59" s="23"/>
       <c r="N59" s="23"/>
-      <c r="O59" s="23"/>
-      <c r="P59" s="22"/>
-      <c r="Q59" s="23"/>
-      <c r="R59" s="22"/>
+      <c r="O59" s="22"/>
+      <c r="P59" s="23"/>
+      <c r="Q59" s="22"/>
+      <c r="R59" s="23"/>
       <c r="S59" s="23"/>
-      <c r="T59" s="23"/>
-      <c r="U59" s="22"/>
-      <c r="V59" s="23"/>
-      <c r="W59" s="22"/>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T59" s="22"/>
+      <c r="U59" s="23"/>
+      <c r="V59" s="22"/>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M60" s="23"/>
       <c r="N60" s="23"/>
-      <c r="O60" s="23"/>
-      <c r="P60" s="22"/>
-      <c r="Q60" s="23"/>
-      <c r="R60" s="22"/>
+      <c r="O60" s="22"/>
+      <c r="P60" s="23"/>
+      <c r="Q60" s="22"/>
+      <c r="R60" s="23"/>
       <c r="S60" s="23"/>
-      <c r="T60" s="23"/>
-      <c r="U60" s="22"/>
-      <c r="V60" s="23"/>
-      <c r="W60" s="22"/>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T60" s="22"/>
+      <c r="U60" s="23"/>
+      <c r="V60" s="22"/>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M61" s="23"/>
       <c r="N61" s="23"/>
-      <c r="O61" s="23"/>
-      <c r="P61" s="22"/>
-      <c r="Q61" s="23"/>
-      <c r="R61" s="22"/>
+      <c r="O61" s="22"/>
+      <c r="P61" s="23"/>
+      <c r="Q61" s="22"/>
+      <c r="R61" s="23"/>
       <c r="S61" s="23"/>
-      <c r="T61" s="23"/>
-      <c r="U61" s="22"/>
-      <c r="V61" s="23"/>
-      <c r="W61" s="22"/>
-    </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T61" s="22"/>
+      <c r="U61" s="23"/>
+      <c r="V61" s="22"/>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M62" s="23"/>
       <c r="N62" s="23"/>
-      <c r="O62" s="23"/>
-      <c r="P62" s="22"/>
-      <c r="Q62" s="23"/>
-      <c r="R62" s="22"/>
+      <c r="O62" s="22"/>
+      <c r="P62" s="23"/>
+      <c r="Q62" s="22"/>
+      <c r="R62" s="23"/>
       <c r="S62" s="23"/>
-      <c r="T62" s="23"/>
-      <c r="U62" s="22"/>
-      <c r="V62" s="23"/>
-      <c r="W62" s="22"/>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T62" s="22"/>
+      <c r="U62" s="23"/>
+      <c r="V62" s="22"/>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M63" s="23"/>
       <c r="N63" s="23"/>
-      <c r="O63" s="23"/>
-      <c r="P63" s="22"/>
-      <c r="Q63" s="23"/>
-      <c r="R63" s="22"/>
+      <c r="O63" s="22"/>
+      <c r="P63" s="23"/>
+      <c r="Q63" s="22"/>
+      <c r="R63" s="23"/>
       <c r="S63" s="23"/>
-      <c r="T63" s="23"/>
-      <c r="U63" s="22"/>
-      <c r="V63" s="23"/>
-      <c r="W63" s="22"/>
-    </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T63" s="22"/>
+      <c r="U63" s="23"/>
+      <c r="V63" s="22"/>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M64" s="23"/>
       <c r="N64" s="23"/>
-      <c r="O64" s="23"/>
-      <c r="P64" s="22"/>
-      <c r="Q64" s="23"/>
-      <c r="R64" s="22"/>
+      <c r="O64" s="22"/>
+      <c r="P64" s="23"/>
+      <c r="Q64" s="22"/>
+      <c r="R64" s="23"/>
       <c r="S64" s="23"/>
-      <c r="T64" s="23"/>
-      <c r="U64" s="22"/>
-      <c r="V64" s="23"/>
-      <c r="W64" s="22"/>
-    </row>
-    <row r="65" spans="14:23" x14ac:dyDescent="0.2">
+      <c r="T64" s="22"/>
+      <c r="U64" s="23"/>
+      <c r="V64" s="22"/>
+    </row>
+    <row r="65" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M65" s="23"/>
       <c r="N65" s="23"/>
-      <c r="O65" s="23"/>
-      <c r="P65" s="22"/>
-      <c r="Q65" s="23"/>
-      <c r="R65" s="22"/>
+      <c r="O65" s="22"/>
+      <c r="P65" s="23"/>
+      <c r="Q65" s="22"/>
+      <c r="R65" s="23"/>
       <c r="S65" s="23"/>
-      <c r="T65" s="23"/>
-      <c r="U65" s="22"/>
-      <c r="V65" s="23"/>
-      <c r="W65" s="22"/>
-    </row>
-    <row r="66" spans="14:23" x14ac:dyDescent="0.2">
+      <c r="T65" s="22"/>
+      <c r="U65" s="23"/>
+      <c r="V65" s="22"/>
+    </row>
+    <row r="66" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M66" s="23"/>
       <c r="N66" s="23"/>
-      <c r="O66" s="23"/>
-      <c r="P66" s="22"/>
-      <c r="Q66" s="23"/>
-      <c r="R66" s="22"/>
+      <c r="O66" s="22"/>
+      <c r="P66" s="23"/>
+      <c r="Q66" s="22"/>
+      <c r="R66" s="23"/>
       <c r="S66" s="23"/>
-      <c r="T66" s="23"/>
-      <c r="U66" s="22"/>
-      <c r="V66" s="23"/>
-      <c r="W66" s="22"/>
-    </row>
-    <row r="67" spans="14:23" x14ac:dyDescent="0.2">
+      <c r="T66" s="22"/>
+      <c r="U66" s="23"/>
+      <c r="V66" s="22"/>
+    </row>
+    <row r="67" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M67" s="23"/>
       <c r="N67" s="23"/>
-      <c r="O67" s="23"/>
-      <c r="P67" s="22"/>
-      <c r="Q67" s="23"/>
-      <c r="R67" s="22"/>
+      <c r="O67" s="22"/>
+      <c r="P67" s="23"/>
+      <c r="Q67" s="22"/>
+      <c r="R67" s="23"/>
       <c r="S67" s="23"/>
-      <c r="T67" s="23"/>
-      <c r="U67" s="22"/>
-      <c r="V67" s="23"/>
-      <c r="W67" s="22"/>
-    </row>
-    <row r="68" spans="14:23" x14ac:dyDescent="0.2">
+      <c r="T67" s="22"/>
+      <c r="U67" s="23"/>
+      <c r="V67" s="22"/>
+    </row>
+    <row r="68" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M68" s="23"/>
       <c r="N68" s="23"/>
-      <c r="O68" s="23"/>
-      <c r="P68" s="22"/>
-      <c r="Q68" s="23"/>
-      <c r="R68" s="22"/>
+      <c r="O68" s="22"/>
+      <c r="P68" s="23"/>
+      <c r="Q68" s="22"/>
+      <c r="R68" s="23"/>
       <c r="S68" s="23"/>
-      <c r="T68" s="23"/>
-      <c r="U68" s="22"/>
-      <c r="V68" s="23"/>
-      <c r="W68" s="22"/>
-    </row>
-    <row r="69" spans="14:23" x14ac:dyDescent="0.2">
+      <c r="T68" s="22"/>
+      <c r="U68" s="23"/>
+      <c r="V68" s="22"/>
+    </row>
+    <row r="69" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M69" s="23"/>
       <c r="N69" s="23"/>
-      <c r="O69" s="23"/>
-      <c r="P69" s="22"/>
-      <c r="Q69" s="23"/>
-      <c r="R69" s="22"/>
+      <c r="O69" s="22"/>
+      <c r="P69" s="23"/>
+      <c r="Q69" s="22"/>
+      <c r="R69" s="23"/>
       <c r="S69" s="23"/>
-      <c r="T69" s="23"/>
-      <c r="U69" s="22"/>
-      <c r="V69" s="23"/>
-      <c r="W69" s="22"/>
-    </row>
-    <row r="70" spans="14:23" x14ac:dyDescent="0.2">
+      <c r="T69" s="22"/>
+      <c r="U69" s="23"/>
+      <c r="V69" s="22"/>
+    </row>
+    <row r="70" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M70" s="23"/>
       <c r="N70" s="23"/>
-      <c r="O70" s="23"/>
-      <c r="P70" s="22"/>
-      <c r="Q70" s="23"/>
-      <c r="R70" s="22"/>
+      <c r="O70" s="22"/>
+      <c r="P70" s="23"/>
+      <c r="Q70" s="22"/>
+      <c r="R70" s="23"/>
       <c r="S70" s="23"/>
-      <c r="T70" s="23"/>
-      <c r="U70" s="22"/>
-      <c r="V70" s="23"/>
-      <c r="W70" s="22"/>
-    </row>
-    <row r="71" spans="14:23" x14ac:dyDescent="0.2">
+      <c r="T70" s="22"/>
+      <c r="U70" s="23"/>
+      <c r="V70" s="22"/>
+    </row>
+    <row r="71" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M71" s="23"/>
       <c r="N71" s="23"/>
-      <c r="O71" s="23"/>
-      <c r="P71" s="22"/>
-      <c r="Q71" s="23"/>
-      <c r="R71" s="22"/>
+      <c r="O71" s="22"/>
+      <c r="P71" s="23"/>
+      <c r="Q71" s="22"/>
+      <c r="R71" s="23"/>
       <c r="S71" s="23"/>
-      <c r="T71" s="23"/>
-      <c r="U71" s="22"/>
-      <c r="V71" s="23"/>
-      <c r="W71" s="22"/>
-    </row>
-    <row r="72" spans="14:23" x14ac:dyDescent="0.2">
+      <c r="T71" s="22"/>
+      <c r="U71" s="23"/>
+      <c r="V71" s="22"/>
+    </row>
+    <row r="72" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M72" s="23"/>
       <c r="N72" s="23"/>
-      <c r="O72" s="23"/>
-      <c r="P72" s="22"/>
-      <c r="Q72" s="23"/>
-      <c r="R72" s="22"/>
+      <c r="O72" s="22"/>
+      <c r="P72" s="23"/>
+      <c r="Q72" s="22"/>
+      <c r="R72" s="23"/>
       <c r="S72" s="23"/>
-      <c r="T72" s="23"/>
-      <c r="U72" s="22"/>
-      <c r="V72" s="23"/>
-      <c r="W72" s="22"/>
-    </row>
-    <row r="73" spans="14:23" x14ac:dyDescent="0.2">
+      <c r="T72" s="22"/>
+      <c r="U72" s="23"/>
+      <c r="V72" s="22"/>
+    </row>
+    <row r="73" spans="13:22" x14ac:dyDescent="0.2">
+      <c r="M73" s="23"/>
       <c r="N73" s="23"/>
-      <c r="O73" s="23"/>
-      <c r="P73" s="22"/>
-      <c r="Q73" s="23"/>
-      <c r="R73" s="22"/>
+      <c r="O73" s="22"/>
+      <c r="P73" s="23"/>
+      <c r="Q73" s="22"/>
+      <c r="R73" s="23"/>
       <c r="S73" s="23"/>
-      <c r="T73" s="23"/>
-      <c r="U73" s="22"/>
-      <c r="V73" s="23"/>
-      <c r="W73" s="22"/>
+      <c r="T73" s="22"/>
+      <c r="U73" s="23"/>
+      <c r="V73" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -22453,7 +22340,7 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="168" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E20" sqref="E20"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22533,17 +22420,17 @@
         <v>10</v>
       </c>
       <c r="B3" s="31">
-        <v>1.1100000000000001E-3</v>
+        <v>2.3E-5</v>
       </c>
       <c r="C3" s="41">
-        <v>1.2160000000000001E-3</v>
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="33"/>
       <c r="F3" s="34"/>
       <c r="G3" s="32"/>
       <c r="H3" s="35">
-        <v>1.0640000000000001E-3</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="I3" s="31">
         <v>1.1069999999999999E-3</v>
@@ -22564,17 +22451,17 @@
         <v>11</v>
       </c>
       <c r="B4" s="31">
-        <v>1.096E-3</v>
+        <v>3.1999999999999999E-5</v>
       </c>
       <c r="C4" s="41">
-        <v>1.15E-3</v>
+        <v>1.7100000000000001E-4</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="33"/>
       <c r="F4" s="34"/>
       <c r="G4" s="32"/>
       <c r="H4" s="35">
-        <v>1.0859999999999999E-3</v>
+        <v>2.5000000000000001E-5</v>
       </c>
       <c r="I4" s="31">
         <v>1.021E-3</v>
@@ -22595,17 +22482,17 @@
         <v>12</v>
       </c>
       <c r="B5" s="31">
-        <v>1.026E-3</v>
+        <v>2.8E-5</v>
       </c>
       <c r="C5" s="41">
-        <v>1.0820000000000001E-3</v>
+        <v>1.08E-4</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="33"/>
       <c r="F5" s="34"/>
       <c r="G5" s="32"/>
       <c r="H5" s="35">
-        <v>1.09E-3</v>
+        <v>2.8E-5</v>
       </c>
       <c r="I5" s="31">
         <v>1.0690000000000001E-3</v>
@@ -22626,17 +22513,17 @@
         <v>13</v>
       </c>
       <c r="B6" s="31">
-        <v>1.0169999999999999E-3</v>
+        <v>2.9E-5</v>
       </c>
       <c r="C6" s="41">
-        <v>1.093E-3</v>
+        <v>1.17E-4</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="33"/>
       <c r="F6" s="34"/>
       <c r="G6" s="32"/>
       <c r="H6" s="35">
-        <v>1.0480000000000001E-3</v>
+        <v>2.9E-5</v>
       </c>
       <c r="I6" s="31">
         <v>1.005E-3</v>
@@ -22657,17 +22544,17 @@
         <v>14</v>
       </c>
       <c r="B7" s="31">
-        <v>1.018E-3</v>
+        <v>3.4E-5</v>
       </c>
       <c r="C7" s="41">
-        <v>1.088E-3</v>
+        <v>1.1400000000000001E-4</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="33"/>
       <c r="F7" s="34"/>
       <c r="G7" s="32"/>
       <c r="H7" s="35">
-        <v>1.039E-3</v>
+        <v>5.5999999999999999E-5</v>
       </c>
       <c r="I7" s="31">
         <v>1.021E-3</v>
@@ -22688,17 +22575,17 @@
         <v>15</v>
       </c>
       <c r="B8" s="31">
-        <v>1.003E-3</v>
+        <v>3.3000000000000003E-5</v>
       </c>
       <c r="C8" s="41">
-        <v>1.075E-3</v>
+        <v>1.17E-4</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="33"/>
       <c r="F8" s="34"/>
       <c r="G8" s="32"/>
       <c r="H8" s="35">
-        <v>9.9500000000000001E-4</v>
+        <v>3.4E-5</v>
       </c>
       <c r="I8" s="31">
         <v>1.0889999999999999E-3</v>
@@ -22719,17 +22606,17 @@
         <v>16</v>
       </c>
       <c r="B9" s="31">
-        <v>9.8400000000000007E-4</v>
+        <v>3.4E-5</v>
       </c>
       <c r="C9" s="41">
-        <v>1.0889999999999999E-3</v>
+        <v>1.2400000000000001E-4</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="33"/>
       <c r="F9" s="34"/>
       <c r="G9" s="32"/>
       <c r="H9" s="35">
-        <v>9.6900000000000003E-4</v>
+        <v>3.3000000000000003E-5</v>
       </c>
       <c r="I9" s="31">
         <v>1.0059999999999999E-3</v>
@@ -22750,17 +22637,17 @@
         <v>17</v>
       </c>
       <c r="B10" s="31">
-        <v>9.7499999999999996E-4</v>
+        <v>3.6999999999999998E-5</v>
       </c>
       <c r="C10" s="41">
-        <v>1.096E-3</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="33"/>
       <c r="F10" s="34"/>
       <c r="G10" s="32"/>
       <c r="H10" s="35">
-        <v>9.1500000000000001E-4</v>
+        <v>3.4E-5</v>
       </c>
       <c r="I10" s="31">
         <v>1.0139999999999999E-3</v>
@@ -22781,17 +22668,17 @@
         <v>18</v>
       </c>
       <c r="B11" s="31">
-        <v>9.4700000000000003E-4</v>
+        <v>4.6999999999999997E-5</v>
       </c>
       <c r="C11" s="41">
-        <v>1.024E-3</v>
+        <v>1.3300000000000001E-4</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="33"/>
       <c r="F11" s="34"/>
       <c r="G11" s="32"/>
       <c r="H11" s="35">
-        <v>9.3700000000000001E-4</v>
+        <v>4.3000000000000002E-5</v>
       </c>
       <c r="I11" s="31">
         <v>9.6199999999999996E-4</v>
@@ -22812,17 +22699,17 @@
         <v>19</v>
       </c>
       <c r="B12" s="31">
-        <v>9.0600000000000001E-4</v>
+        <v>3.6999999999999998E-5</v>
       </c>
       <c r="C12" s="41">
-        <v>1.124E-3</v>
+        <v>1.34E-4</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="33"/>
       <c r="F12" s="34"/>
       <c r="G12" s="32"/>
       <c r="H12" s="35">
-        <v>9.5399999999999999E-4</v>
+        <v>3.4999999999999997E-5</v>
       </c>
       <c r="I12" s="31">
         <v>9.68E-4</v>
@@ -22843,17 +22730,17 @@
         <v>20</v>
       </c>
       <c r="B13" s="31">
-        <v>9.1500000000000001E-4</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="C13" s="41">
-        <v>1.07E-3</v>
+        <v>1.35E-4</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="33"/>
       <c r="F13" s="34"/>
       <c r="G13" s="32"/>
       <c r="H13" s="35">
-        <v>9.5799999999999998E-4</v>
+        <v>3.8999999999999999E-5</v>
       </c>
       <c r="I13" s="31">
         <v>1.031E-3</v>
@@ -22874,17 +22761,17 @@
         <v>21</v>
       </c>
       <c r="B14" s="31">
-        <v>9.7300000000000002E-4</v>
+        <v>3.8999999999999999E-5</v>
       </c>
       <c r="C14" s="41">
-        <v>1.0579999999999999E-3</v>
+        <v>1.4200000000000001E-4</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="33"/>
       <c r="F14" s="34"/>
       <c r="G14" s="32"/>
       <c r="H14" s="35">
-        <v>9.1200000000000005E-4</v>
+        <v>3.1999999999999999E-5</v>
       </c>
       <c r="I14" s="31">
         <v>9.6599999999999995E-4</v>
@@ -22905,17 +22792,17 @@
         <v>22</v>
       </c>
       <c r="B15" s="31">
-        <v>9.3899999999999995E-4</v>
+        <v>3.8000000000000002E-5</v>
       </c>
       <c r="C15" s="41">
-        <v>1.024E-3</v>
+        <v>1.5200000000000001E-4</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="33"/>
       <c r="F15" s="34"/>
       <c r="G15" s="32"/>
       <c r="H15" s="35">
-        <v>9.1500000000000001E-4</v>
+        <v>3.1999999999999999E-5</v>
       </c>
       <c r="I15" s="31">
         <v>9.2599999999999996E-4</v>
@@ -22936,17 +22823,17 @@
         <v>23</v>
       </c>
       <c r="B16" s="31">
-        <v>9.3099999999999997E-4</v>
+        <v>3.8999999999999999E-5</v>
       </c>
       <c r="C16" s="41">
-        <v>1.005E-3</v>
+        <v>1.5899999999999999E-4</v>
       </c>
       <c r="D16" s="32"/>
       <c r="E16" s="33"/>
       <c r="F16" s="34"/>
       <c r="G16" s="32"/>
       <c r="H16" s="35">
-        <v>9.0499999999999999E-4</v>
+        <v>3.6999999999999998E-5</v>
       </c>
       <c r="I16" s="31">
         <v>9.3000000000000005E-4</v>
@@ -22967,17 +22854,17 @@
         <v>24</v>
       </c>
       <c r="B17" s="31">
-        <v>9.0300000000000005E-4</v>
+        <v>4.1E-5</v>
       </c>
       <c r="C17" s="41">
-        <v>1.0480000000000001E-3</v>
+        <v>1.5699999999999999E-4</v>
       </c>
       <c r="D17" s="32"/>
       <c r="E17" s="33"/>
       <c r="F17" s="34"/>
       <c r="G17" s="32"/>
       <c r="H17" s="35">
-        <v>8.8000000000000003E-4</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="I17" s="31">
         <v>9.5600000000000004E-4</v>
@@ -22998,17 +22885,17 @@
         <v>25</v>
       </c>
       <c r="B18" s="31">
-        <v>9.2500000000000004E-4</v>
+        <v>4.1999999999999998E-5</v>
       </c>
       <c r="C18" s="41">
-        <v>1.036E-3</v>
+        <v>1.66E-4</v>
       </c>
       <c r="D18" s="32"/>
       <c r="E18" s="33"/>
       <c r="F18" s="34"/>
       <c r="G18" s="32"/>
       <c r="H18" s="35">
-        <v>8.8999999999999995E-4</v>
+        <v>3.4999999999999997E-5</v>
       </c>
       <c r="I18" s="31">
         <v>9.0300000000000005E-4</v>
@@ -23029,17 +22916,17 @@
         <v>26</v>
       </c>
       <c r="B19" s="31">
-        <v>9.1200000000000005E-4</v>
+        <v>4.5000000000000003E-5</v>
       </c>
       <c r="C19" s="41">
-        <v>1.024E-3</v>
+        <v>1.7200000000000001E-4</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="33"/>
       <c r="F19" s="34"/>
       <c r="G19" s="32"/>
       <c r="H19" s="35">
-        <v>8.0699999999999999E-4</v>
+        <v>3.8000000000000002E-5</v>
       </c>
       <c r="I19" s="31">
         <v>9.5399999999999999E-4</v>
@@ -23060,17 +22947,17 @@
         <v>27</v>
       </c>
       <c r="B20" s="31">
-        <v>8.7500000000000002E-4</v>
+        <v>4.8000000000000001E-5</v>
       </c>
       <c r="C20" s="41">
-        <v>9.990000000000001E-4</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="33"/>
       <c r="F20" s="34"/>
       <c r="G20" s="32"/>
       <c r="H20" s="35">
-        <v>7.7300000000000003E-4</v>
+        <v>3.8999999999999999E-5</v>
       </c>
       <c r="I20" s="31">
         <v>9.0899999999999998E-4</v>
@@ -23091,17 +22978,17 @@
         <v>28</v>
       </c>
       <c r="B21" s="31">
-        <v>9.0700000000000004E-4</v>
+        <v>4.8000000000000001E-5</v>
       </c>
       <c r="C21" s="41">
-        <v>1.026E-3</v>
+        <v>2.23E-4</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="33"/>
       <c r="F21" s="34"/>
       <c r="G21" s="32"/>
       <c r="H21" s="35">
-        <v>7.2599999999999997E-4</v>
+        <v>3.8000000000000002E-5</v>
       </c>
       <c r="I21" s="31">
         <v>8.7699999999999996E-4</v>
@@ -23122,17 +23009,17 @@
         <v>29</v>
       </c>
       <c r="B22" s="31">
-        <v>8.9899999999999995E-4</v>
+        <v>4.8999999999999998E-5</v>
       </c>
       <c r="C22" s="41">
-        <v>1.0200000000000001E-3</v>
+        <v>1.94E-4</v>
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="33"/>
       <c r="F22" s="34"/>
       <c r="G22" s="32"/>
       <c r="H22" s="35">
-        <v>7.7999999999999999E-4</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="I22" s="31">
         <v>8.8900000000000003E-4</v>
@@ -23153,17 +23040,17 @@
         <v>30</v>
       </c>
       <c r="B23" s="31">
-        <v>8.8599999999999996E-4</v>
+        <v>4.3999999999999999E-5</v>
       </c>
       <c r="C23" s="41">
-        <v>1.005E-3</v>
+        <v>2.03E-4</v>
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="33"/>
       <c r="F23" s="34"/>
       <c r="G23" s="32"/>
       <c r="H23" s="35">
-        <v>7.3800000000000005E-4</v>
+        <v>6.4999999999999994E-5</v>
       </c>
       <c r="I23" s="31">
         <v>9.1100000000000003E-4</v>
@@ -23184,17 +23071,17 @@
         <v>31</v>
       </c>
       <c r="B24" s="31">
-        <v>9.2199999999999997E-4</v>
+        <v>4.3999999999999999E-5</v>
       </c>
       <c r="C24" s="41">
-        <v>1.016E-3</v>
+        <v>2.0699999999999999E-4</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="33"/>
       <c r="F24" s="34"/>
       <c r="G24" s="32"/>
       <c r="H24" s="35">
-        <v>7.4100000000000001E-4</v>
+        <v>4.3999999999999999E-5</v>
       </c>
       <c r="I24" s="31">
         <v>9.0700000000000004E-4</v>
@@ -23215,17 +23102,17 @@
         <v>32</v>
       </c>
       <c r="B25" s="31">
-        <v>8.8400000000000002E-4</v>
+        <v>4.6E-5</v>
       </c>
       <c r="C25" s="41">
-        <v>9.9200000000000004E-4</v>
+        <v>2.22E-4</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="33"/>
       <c r="F25" s="34"/>
       <c r="G25" s="32"/>
       <c r="H25" s="35">
-        <v>7.4899999999999999E-4</v>
+        <v>4.3999999999999999E-5</v>
       </c>
       <c r="I25" s="31">
         <v>9.2000000000000003E-4</v>
@@ -23246,17 +23133,17 @@
         <v>50</v>
       </c>
       <c r="B26" s="31">
-        <v>8.7900000000000001E-4</v>
+        <v>7.8999999999999996E-5</v>
       </c>
       <c r="C26" s="41">
-        <v>1.106E-3</v>
+        <v>3.68E-4</v>
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="33"/>
       <c r="F26" s="34"/>
       <c r="G26" s="32"/>
       <c r="H26" s="35">
-        <v>7.5900000000000002E-4</v>
+        <v>6.3E-5</v>
       </c>
       <c r="I26" s="31">
         <v>9.3099999999999997E-4</v>
@@ -23277,17 +23164,17 @@
         <v>100</v>
       </c>
       <c r="B27" s="31">
-        <v>8.8500000000000004E-4</v>
+        <v>2.1800000000000001E-4</v>
       </c>
       <c r="C27" s="41">
-        <v>1.3500000000000001E-3</v>
+        <v>8.4800000000000001E-4</v>
       </c>
       <c r="D27" s="32"/>
       <c r="E27" s="33"/>
       <c r="F27" s="34"/>
       <c r="G27" s="32"/>
       <c r="H27" s="35">
-        <v>7.3899999999999997E-4</v>
+        <v>1.17E-4</v>
       </c>
       <c r="I27" s="31">
         <v>8.9099999999999997E-4</v>
@@ -23308,17 +23195,17 @@
         <v>200</v>
       </c>
       <c r="B28" s="31">
-        <v>1.3240000000000001E-3</v>
+        <v>6.7199999999999996E-4</v>
       </c>
       <c r="C28" s="41">
-        <v>2.3509999999999998E-3</v>
+        <v>2.1710000000000002E-3</v>
       </c>
       <c r="D28" s="32"/>
       <c r="E28" s="33"/>
       <c r="F28" s="34"/>
       <c r="G28" s="32"/>
       <c r="H28" s="35">
-        <v>7.6999999999999996E-4</v>
+        <v>2.2599999999999999E-4</v>
       </c>
       <c r="I28" s="31">
         <v>8.7399999999999999E-4</v>
@@ -23339,17 +23226,17 @@
         <v>500</v>
       </c>
       <c r="B29" s="31">
-        <v>3.9870000000000001E-3</v>
+        <v>3.555E-3</v>
       </c>
       <c r="C29" s="41">
-        <v>7.9150000000000002E-3</v>
+        <v>9.7920000000000004E-3</v>
       </c>
       <c r="D29" s="32"/>
       <c r="E29" s="33"/>
       <c r="F29" s="34"/>
       <c r="G29" s="32"/>
       <c r="H29" s="35">
-        <v>8.0099999999999995E-4</v>
+        <v>5.3200000000000003E-4</v>
       </c>
       <c r="I29" s="31">
         <v>7.9900000000000001E-4</v>
@@ -23370,17 +23257,17 @@
         <v>1000</v>
       </c>
       <c r="B30" s="31">
-        <v>1.4024E-2</v>
+        <v>1.3431E-2</v>
       </c>
       <c r="C30" s="41">
-        <v>2.5225000000000001E-2</v>
+        <v>3.0678E-2</v>
       </c>
       <c r="D30" s="32"/>
       <c r="E30" s="33"/>
       <c r="F30" s="34"/>
       <c r="G30" s="32"/>
       <c r="H30" s="35">
-        <v>9.5100000000000002E-4</v>
+        <v>9.3899999999999995E-4</v>
       </c>
       <c r="I30" s="31">
         <v>8.3199999999999995E-4</v>
@@ -23401,17 +23288,17 @@
         <v>1500</v>
       </c>
       <c r="B31" s="31">
-        <v>3.0928000000000001E-2</v>
+        <v>3.0391000000000001E-2</v>
       </c>
       <c r="C31" s="41">
-        <v>5.4580999999999998E-2</v>
+        <v>5.6461999999999998E-2</v>
       </c>
       <c r="D31" s="32"/>
       <c r="E31" s="33"/>
       <c r="F31" s="34"/>
       <c r="G31" s="32"/>
       <c r="H31" s="35">
-        <v>9.9299999999999996E-4</v>
+        <v>3.8630000000000001E-3</v>
       </c>
       <c r="I31" s="31">
         <v>8.6600000000000002E-4</v>
@@ -23432,17 +23319,17 @@
         <v>2000</v>
       </c>
       <c r="B32" s="31">
-        <v>5.2406000000000001E-2</v>
+        <v>5.6461999999999998E-2</v>
       </c>
       <c r="C32" s="41">
-        <v>9.3287999999999996E-2</v>
+        <v>9.4612000000000002E-2</v>
       </c>
       <c r="D32" s="32"/>
       <c r="E32" s="33"/>
       <c r="F32" s="34"/>
       <c r="G32" s="32"/>
       <c r="H32" s="35">
-        <v>1.225E-3</v>
+        <v>4.4019999999999997E-3</v>
       </c>
       <c r="I32" s="31">
         <v>8.8900000000000003E-4</v>
@@ -23463,17 +23350,17 @@
         <v>2500</v>
       </c>
       <c r="B33" s="31">
-        <v>8.0239000000000005E-2</v>
+        <v>8.3535999999999999E-2</v>
       </c>
       <c r="C33" s="41">
-        <v>0.14021800000000001</v>
+        <v>0.146647</v>
       </c>
       <c r="D33" s="32"/>
       <c r="E33" s="33"/>
       <c r="F33" s="34"/>
       <c r="G33" s="32"/>
       <c r="H33" s="35">
-        <v>1.3290000000000001E-3</v>
+        <v>4.7229999999999998E-3</v>
       </c>
       <c r="I33" s="31">
         <v>1.0280000000000001E-3</v>
@@ -23494,17 +23381,17 @@
         <v>5000</v>
       </c>
       <c r="B34" s="31">
-        <v>0.32545299999999999</v>
+        <v>0.33501500000000001</v>
       </c>
       <c r="C34" s="41">
-        <v>0.55376599999999998</v>
+        <v>0.53937100000000004</v>
       </c>
       <c r="D34" s="32"/>
       <c r="E34" s="33"/>
       <c r="F34" s="34"/>
       <c r="G34" s="32"/>
       <c r="H34" s="35">
-        <v>1.807E-3</v>
+        <v>1.0980999999999999E-2</v>
       </c>
       <c r="I34" s="31">
         <v>1.067E-3</v>
@@ -23525,17 +23412,17 @@
         <v>10000</v>
       </c>
       <c r="B35" s="31">
-        <v>1.3117840000000001</v>
+        <v>1.2789299999999999</v>
       </c>
       <c r="C35" s="41">
-        <v>2.246</v>
+        <v>2.26553</v>
       </c>
       <c r="D35" s="32"/>
       <c r="E35" s="33"/>
       <c r="F35" s="34"/>
       <c r="G35" s="32"/>
       <c r="H35" s="35">
-        <v>4.6280000000000002E-3</v>
+        <v>2.8652E-2</v>
       </c>
       <c r="I35" s="31">
         <v>1.6739999999999999E-3</v>
@@ -23556,17 +23443,17 @@
         <v>20000</v>
       </c>
       <c r="B36" s="31">
-        <v>5.0392570000000001</v>
+        <v>5.3461790000000002</v>
       </c>
       <c r="C36" s="41">
-        <v>8.7627050000000004</v>
+        <v>9.6585999999999999</v>
       </c>
       <c r="D36" s="32"/>
       <c r="E36" s="33"/>
       <c r="F36" s="34"/>
       <c r="G36" s="32"/>
       <c r="H36" s="35">
-        <v>8.7150000000000005E-3</v>
+        <v>6.4096E-2</v>
       </c>
       <c r="I36" s="31">
         <v>2.8670000000000002E-3</v>
@@ -23587,17 +23474,17 @@
         <v>30000</v>
       </c>
       <c r="B37" s="31">
-        <v>11.962857</v>
+        <v>12.795745</v>
       </c>
       <c r="C37" s="41">
-        <v>19.352063000000001</v>
+        <v>20.059473000000001</v>
       </c>
       <c r="D37" s="32"/>
       <c r="E37" s="33"/>
       <c r="F37" s="34"/>
       <c r="G37" s="32"/>
       <c r="H37" s="35">
-        <v>1.1431999999999999E-2</v>
+        <v>0.100523</v>
       </c>
       <c r="I37" s="31">
         <v>4.5459999999999997E-3</v>
@@ -23618,17 +23505,17 @@
         <v>40000</v>
       </c>
       <c r="B38" s="31">
-        <v>20.429576999999998</v>
+        <v>22.261482000000001</v>
       </c>
       <c r="C38" s="41">
-        <v>35.314757</v>
+        <v>36.508553999999997</v>
       </c>
       <c r="D38" s="32"/>
       <c r="E38" s="33"/>
       <c r="F38" s="34"/>
       <c r="G38" s="32"/>
       <c r="H38" s="35">
-        <v>1.4711999999999999E-2</v>
+        <v>0.13483400000000001</v>
       </c>
       <c r="I38" s="31">
         <v>5.2680000000000001E-3</v>
@@ -23649,17 +23536,17 @@
         <v>50000</v>
       </c>
       <c r="B39" s="31">
-        <v>33.108294999999998</v>
+        <v>36.279274999999998</v>
       </c>
       <c r="C39" s="41">
-        <v>53.302705000000003</v>
+        <v>54.648324000000002</v>
       </c>
       <c r="D39" s="32"/>
       <c r="E39" s="33"/>
       <c r="F39" s="34"/>
       <c r="G39" s="32"/>
       <c r="H39" s="35">
-        <v>1.7330999999999999E-2</v>
+        <v>0.19148200000000001</v>
       </c>
       <c r="I39" s="31">
         <v>9.1339999999999998E-3</v>
@@ -24290,7 +24177,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
@@ -24299,7 +24186,7 @@
       <c r="G1" s="49"/>
       <c r="H1" s="50"/>
       <c r="I1" s="51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" s="52"/>
       <c r="K1" s="52"/>

</xml_diff>